<commit_message>
Auto-committed on 2022/03/31 週四
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/CustDataCtrl.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/CustDataCtrl.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27AB8B5-2F33-4618-97D1-6077CBF21B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D283042D-9EFC-4AFC-9D78-FFA41BD3DB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="240" yWindow="384" windowWidth="22800" windowHeight="11976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>讀取Key條件</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -290,6 +290,42 @@
   </si>
   <si>
     <t>客戶申請留存原始戶名用 by eric 2022.3.25</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetDate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>設定日期</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>設定人員</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReSetDate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除日期</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除人員</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>by eric 2022.3.31</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReSetEmpNo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetEmpNo</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -385,7 +421,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +437,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,7 +508,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -524,17 +566,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -876,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -894,10 +942,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="8" t="s">
         <v>45</v>
       </c>
@@ -909,8 +957,8 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="12" t="s">
         <v>39</v>
       </c>
@@ -922,10 +970,10 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="8" t="s">
         <v>29</v>
       </c>
@@ -935,10 +983,10 @@
       <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="15" t="s">
         <v>34</v>
       </c>
@@ -950,10 +998,10 @@
       <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16"/>
       <c r="E5" s="14"/>
@@ -961,10 +1009,10 @@
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="15"/>
       <c r="D6" s="16"/>
       <c r="E6" s="14"/>
@@ -972,10 +1020,10 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
       <c r="E7" s="14"/>
@@ -1043,7 +1091,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" ht="81" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>3</v>
       </c>
@@ -1087,20 +1135,20 @@
       <c r="A13" s="18">
         <v>5</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="20">
         <v>10</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1108,20 +1156,20 @@
       <c r="A14" s="18">
         <v>6</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="20">
         <v>100</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21" t="s">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1129,107 +1177,155 @@
       <c r="A15" s="18">
         <v>7</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="B15" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="22">
+        <v>8</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>8</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="18" t="s">
+      <c r="B16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="21">
         <v>6</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>9</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="B17" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="22">
+        <v>8</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>10</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="18">
+      <c r="B18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="21">
         <v>6</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="18">
+        <v>11</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="A20" s="18">
+        <v>12</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="18">
+        <v>6</v>
+      </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="A21" s="18">
+        <v>13</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
+      <c r="A22" s="18">
+        <v>14</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="18">
+        <v>6</v>
+      </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
     </row>
@@ -1718,6 +1814,42 @@
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
       <c r="G76" s="18"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="18"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Auto-committed on 2023/03/24 週五 17:19:08.22
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/CustDataCtrl.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/CustDataCtrl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31D2833-90A7-4DA6-9099-EACA257C0F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BAF7B6-B46C-4037-B444-E76BD5FBB750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
   <si>
     <t>讀取Key條件</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -365,6 +365,18 @@
   <si>
     <t>ApplMark ^i</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXCustId</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>申請後身份證字號/統一編號</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>客戶申請後留存變更後ID by Mata 2023.3.23</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -467,7 +479,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,6 +501,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,7 +575,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -626,6 +644,12 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -968,17 +992,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.5546875" style="3" customWidth="1"/>
@@ -1221,19 +1245,21 @@
       <c r="A15" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19" t="s">
-        <v>60</v>
+      <c r="B15" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="24">
+        <v>10</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1241,17 +1267,15 @@
         <v>8</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="19">
-        <v>6</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="20"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19" t="s">
         <v>60</v>
@@ -1262,15 +1286,17 @@
         <v>9</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="19">
+        <v>6</v>
+      </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19" t="s">
         <v>60</v>
@@ -1281,17 +1307,15 @@
         <v>10</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="19">
-        <v>6</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="20"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19" t="s">
         <v>60</v>
@@ -1301,35 +1325,37 @@
       <c r="A19" s="16">
         <v>11</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="B19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="19">
+        <v>6</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>12</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="16">
-        <v>6</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
@@ -1338,15 +1364,17 @@
         <v>13</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="E21" s="16">
+        <v>6</v>
+      </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
@@ -1355,26 +1383,34 @@
         <v>14</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="16">
-        <v>6</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
+      <c r="A23" s="1">
+        <v>15</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="16">
+        <v>6</v>
+      </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
@@ -1890,6 +1926,15 @@
       <c r="E80" s="16"/>
       <c r="F80" s="16"/>
       <c r="G80" s="16"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1911,7 +1956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>

</xml_diff>